<commit_message>
Setup listview to only display groupings
</commit_message>
<xml_diff>
--- a/File Import/Ingredient .xlsx
+++ b/File Import/Ingredient .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ut-info6.OMAG\Desktop\ProgettoPrins\File Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ut-info6.OMAG\source\repos\StorageManager\File Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E67A2D7-0D34-4CC8-B91E-F515904C2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B1ED4F-D16C-4612-81C9-82E69397BD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16080" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{93B019CF-B113-4B0E-B0D6-654848969CA6}"/>
   </bookViews>
@@ -1656,7 +1656,7 @@
   <dimension ref="A1:I367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D370" sqref="D370"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>